<commit_message>
MERN stack  --Ensaf Library web app done --
</commit_message>
<xml_diff>
--- a/server/assets/test.xlsx
+++ b/server/assets/test.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="114">
   <si>
     <t>id</t>
   </si>
@@ -31,56 +31,338 @@
     <t>isAdmin</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>user1@example.com</t>
-  </si>
-  <si>
-    <t>password1</t>
-  </si>
-  <si>
-    <t>nacer</t>
-  </si>
-  <si>
-    <t>user2@example.com</t>
-  </si>
-  <si>
-    <t>password2</t>
-  </si>
-  <si>
-    <t>imane</t>
-  </si>
-  <si>
-    <t>user3@example.com</t>
-  </si>
-  <si>
-    <t>password3</t>
-  </si>
-  <si>
-    <t>Admin2</t>
-  </si>
-  <si>
-    <t>user4@example.com</t>
-  </si>
-  <si>
-    <t>password4</t>
-  </si>
-  <si>
-    <t>Ibno roched</t>
-  </si>
-  <si>
-    <t>use@example.com</t>
-  </si>
-  <si>
-    <t>passwor</t>
+    <t>False</t>
+  </si>
+  <si>
+    <t>onganiso.zulu@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>ZULU ONGANISO</t>
+  </si>
+  <si>
+    <t>hajar.touti@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>TOUTI HAJAR</t>
+  </si>
+  <si>
+    <t>hanane.talhaoui@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>TALHAOUI HANANE</t>
+  </si>
+  <si>
+    <t>hanae.sbai@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>SBAI HANAE</t>
+  </si>
+  <si>
+    <t>nada.salbi@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>SALBI NADA</t>
+  </si>
+  <si>
+    <t>aida.rami@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>RAMI AIDA</t>
+  </si>
+  <si>
+    <t>deyae.ouazzanitaybi@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>OUAZZANI TAYBI  DEYAE</t>
+  </si>
+  <si>
+    <t>ibtissame.oumahrir@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>OU-MAHRIR IBTISSAME</t>
+  </si>
+  <si>
+    <t>junior.ndomaletina@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>NDOMALE TINA JUNIOR</t>
+  </si>
+  <si>
+    <t>rim.moujtahid@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>MOUJTAHID RIM</t>
+  </si>
+  <si>
+    <t>vianney.mbaallogo@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>MBA ALLOGO VIANNEY</t>
+  </si>
+  <si>
+    <t>omar.makroum@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>MAKROUM OMAR</t>
+  </si>
+  <si>
+    <t>mohammed.majid@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAJID MOHAMMED </t>
+  </si>
+  <si>
+    <t>tarik.machlaf@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>MACHLAF TARIK</t>
+  </si>
+  <si>
+    <t>oumaima.lyousfi@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>LYOUSFI OUMAIMA</t>
+  </si>
+  <si>
+    <t>abdelilah.laksir@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>LAKSIR ABDELILAH</t>
+  </si>
+  <si>
+    <t>sara.lahlou3@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>LAHLOU SARA</t>
+  </si>
+  <si>
+    <t>kelvis.kaunda@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>KAUNDA KELVIS</t>
+  </si>
+  <si>
+    <t>hind.guendouz@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>GUENDOUZ  HIND</t>
+  </si>
+  <si>
+    <t>ismail.fathi1@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>FATHI ISMAIL</t>
+  </si>
+  <si>
+    <t>fatimazahrae.elfoghali@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>EL FOGHALI FATIMA ZAHRAE</t>
+  </si>
+  <si>
+    <t>nacreddine.chouich@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>CHOUICH  NACEREDDINE</t>
+  </si>
+  <si>
+    <t>kawtar.chkoubi@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>CHKOUBI KAWTAR</t>
+  </si>
+  <si>
+    <t>younessaidali.bourhane@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOURHANE YOUNES SAID ALI </t>
+  </si>
+  <si>
+    <t>alyazid.bouchiba@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>BOUCHIBA AL YAZID</t>
+  </si>
+  <si>
+    <t>houssam.bouardi@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>BOUARDI HOUSSAM</t>
+  </si>
+  <si>
+    <t>meryem.beraida@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>BERAIDA MERYEM</t>
+  </si>
+  <si>
+    <t>ayoub.benali@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>BEN ALI AYOUB</t>
+  </si>
+  <si>
+    <t>imane.arioua@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>ARIOUA IMANE</t>
+  </si>
+  <si>
+    <t>salma.aqil@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>AQIL SALMA</t>
+  </si>
+  <si>
+    <t>naima.ammar@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>AMMAR NAIMA</t>
+  </si>
+  <si>
+    <t>asmae.amakrane@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>AMAKRANE ASMAE</t>
+  </si>
+  <si>
+    <t>salma.alaouiismaili1@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>ALAOUI ISMAILI SALMA</t>
+  </si>
+  <si>
+    <t>walid.akkoujane@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>AKKOUJANE WALID</t>
+  </si>
+  <si>
+    <t>assia.aitelkadi@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>AITELKADI ASSIA</t>
+  </si>
+  <si>
+    <t>mohamed.agoumi@usmba.ac.ma</t>
+  </si>
+  <si>
+    <t>AGOUMI MOHAMED</t>
+  </si>
+  <si>
+    <t>8p#h3nPIF99!</t>
+  </si>
+  <si>
+    <t>HJhR77Iu^9lT</t>
+  </si>
+  <si>
+    <t>yZ3V50*VQk4s</t>
+  </si>
+  <si>
+    <t>7nE#4uj&amp;5Y0Y</t>
+  </si>
+  <si>
+    <t>46R%h5$pUsyQ</t>
+  </si>
+  <si>
+    <t>245RP49Ozfd!</t>
+  </si>
+  <si>
+    <t>INVk7i$^4wm1</t>
+  </si>
+  <si>
+    <t>A#7M5ZVU6Qgi</t>
+  </si>
+  <si>
+    <t>Zz71F%dWetc5</t>
+  </si>
+  <si>
+    <t>Tj$1^q89caeG</t>
+  </si>
+  <si>
+    <t>6Gw3JhF76Q!k</t>
+  </si>
+  <si>
+    <t>7jAqos&amp;E25E#</t>
+  </si>
+  <si>
+    <t>18cCIBgd3j*$</t>
+  </si>
+  <si>
+    <t>6i2R!631YxH&amp;</t>
+  </si>
+  <si>
+    <t>g3*f9QtFW3Z8</t>
+  </si>
+  <si>
+    <t>4T%*jv3Rm2Yz</t>
+  </si>
+  <si>
+    <t>9dHeP18!865U</t>
+  </si>
+  <si>
+    <t>94$0rBF4rNii</t>
+  </si>
+  <si>
+    <t>bTIS1^8t%9X6</t>
+  </si>
+  <si>
+    <t>7Ol1u*Vn^8s$</t>
+  </si>
+  <si>
+    <t>C4D%d6asep7r</t>
+  </si>
+  <si>
+    <t>M2a^BZE3!5L4</t>
+  </si>
+  <si>
+    <t>79ojul9#O3eI</t>
+  </si>
+  <si>
+    <t>t9A^0w9tu8*x</t>
+  </si>
+  <si>
+    <t>7#7w3&amp;cEVa4^</t>
+  </si>
+  <si>
+    <t>DJEwx!6t58Wq</t>
+  </si>
+  <si>
+    <t>D^4J83NTPQWc</t>
+  </si>
+  <si>
+    <t>Tuh66uIb62K!</t>
+  </si>
+  <si>
+    <t>rqz3e9Z&amp;h0lj</t>
+  </si>
+  <si>
+    <t>*X^7zqL48AhB</t>
+  </si>
+  <si>
+    <t>HFsr4&amp;8mY&amp;C1</t>
+  </si>
+  <si>
+    <t>g06a5YgRw**0</t>
+  </si>
+  <si>
+    <t>tjaM090d27!^</t>
+  </si>
+  <si>
+    <t>w0&amp;ChZK79&amp;R^</t>
+  </si>
+  <si>
+    <t>38!bEwkJyS6F</t>
+  </si>
+  <si>
+    <t>3488yO7Pcg!9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,6 +378,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,7 +401,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -113,14 +409,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -458,123 +782,683 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34.5" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="4" max="4" width="21.875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="E6">
-        <v>0</v>
+      <c r="B20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId1" display="cO@q2J5SQ81g"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:E5 A6 E6" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>